<commit_message>
Atualização slides (bordas também)
</commit_message>
<xml_diff>
--- a/documentacao/P&I/gestao de riscos.xlsx
+++ b/documentacao/P&I/gestao de riscos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\Repositorios\sdpiar\documentacao\P&amp;I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\sdpiar\documentacao\P&amp;I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F63CEF64-DC68-4201-A7E3-7DE8060EEA51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF82710C-C4CB-4DEB-A4E4-4868FE420171}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -112,13 +111,16 @@
   </si>
   <si>
     <t>1 dia</t>
+  </si>
+  <si>
+    <t>Controle de Riscos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +128,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -190,13 +211,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -205,9 +224,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -221,9 +238,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -233,21 +248,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,6 +290,112 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>277815</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4817</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B57008BF-C902-4847-8E6D-0BB86C2ED6D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700003" y="476251"/>
+          <a:ext cx="277810" cy="235004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1022629</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>420690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C5654A8-E678-43B2-8F6A-19AD4A36AB7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3182938" y="63502"/>
+          <a:ext cx="959129" cy="357188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A62A1B8-29AB-48F1-A3C3-532BE985E7DC}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,171 +709,185 @@
     <col min="7" max="7" width="90.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H3" s="11" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1"/>
+      <c r="F5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="F6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>